<commit_message>
stickers, cards, purchase recs, supplies
edited the mentioned files
</commit_message>
<xml_diff>
--- a/Supplies.xlsx
+++ b/Supplies.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8952" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="8952"/>
   </bookViews>
   <sheets>
     <sheet name="Capital Estimate (Inspired)" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="129">
   <si>
     <t>Quantity</t>
   </si>
@@ -265,6 +265,9 @@
     <t>copaiba</t>
   </si>
   <si>
+    <t>sage</t>
+  </si>
+  <si>
     <t>tea tree</t>
   </si>
   <si>
@@ -301,7 +304,16 @@
     <t>turmeric</t>
   </si>
   <si>
-    <t>spearmint</t>
+    <t>peppermint</t>
+  </si>
+  <si>
+    <t>black pepper</t>
+  </si>
+  <si>
+    <t>tulip</t>
+  </si>
+  <si>
+    <t>lemongrass</t>
   </si>
   <si>
     <t>vetiver</t>
@@ -1150,7 +1162,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1310,20 +1322,14 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1805,8 +1811,8 @@
   <sheetPr/>
   <dimension ref="A1:G1012"/>
   <sheetViews>
-    <sheetView zoomScale="82" zoomScaleNormal="82" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="H68" sqref="H68"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4298245614035" defaultRowHeight="15" customHeight="1" outlineLevelCol="6"/>
@@ -2759,7 +2765,7 @@
         <v>20</v>
       </c>
       <c r="D57" s="49">
-        <f t="shared" ref="D57:D66" si="1">B57*C57</f>
+        <f t="shared" ref="D57:D68" si="1">B57*C57</f>
         <v>1000</v>
       </c>
       <c r="E57" s="5" t="s">
@@ -2788,16 +2794,16 @@
       <c r="F58" s="51"/>
     </row>
     <row r="59" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A59" s="49" t="s">
+      <c r="A59" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B59" s="50">
+      <c r="B59" s="44">
         <v>2</v>
       </c>
-      <c r="C59" s="50">
+      <c r="C59" s="44">
         <v>46</v>
       </c>
-      <c r="D59" s="49">
+      <c r="D59" s="17">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
@@ -2810,16 +2816,16 @@
       </c>
     </row>
     <row r="60" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A60" s="52" t="s">
+      <c r="A60" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B60" s="50">
-        <v>1</v>
-      </c>
-      <c r="C60" s="50">
+      <c r="B60" s="44">
+        <v>1</v>
+      </c>
+      <c r="C60" s="44">
         <v>58</v>
       </c>
-      <c r="D60" s="49">
+      <c r="D60" s="17">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
@@ -2827,16 +2833,16 @@
       <c r="F60" s="51"/>
     </row>
     <row r="61" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A61" s="49" t="s">
+      <c r="A61" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B61" s="50">
+      <c r="B61" s="44">
         <v>3</v>
       </c>
-      <c r="C61" s="50">
+      <c r="C61" s="44">
         <v>230</v>
       </c>
-      <c r="D61" s="49">
+      <c r="D61" s="17">
         <f t="shared" si="1"/>
         <v>690</v>
       </c>
@@ -2849,16 +2855,16 @@
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A62" s="52" t="s">
+      <c r="A62" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B62" s="50">
-        <v>1</v>
-      </c>
-      <c r="C62" s="50">
+      <c r="B62" s="44">
+        <v>1</v>
+      </c>
+      <c r="C62" s="44">
         <v>125</v>
       </c>
-      <c r="D62" s="49">
+      <c r="D62" s="17">
         <f t="shared" si="1"/>
         <v>125</v>
       </c>
@@ -2866,80 +2872,83 @@
       <c r="F62" s="51"/>
     </row>
     <row r="63" ht="14.25" customHeight="1" spans="1:7">
-      <c r="A63" t="s">
+      <c r="A63" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B63" s="5">
-        <v>1</v>
-      </c>
-      <c r="C63" s="5">
+      <c r="B63" s="50">
+        <v>1</v>
+      </c>
+      <c r="C63" s="50">
+        <f>520</f>
         <v>520</v>
       </c>
-      <c r="D63" s="53">
+      <c r="D63" s="49">
         <f t="shared" si="1"/>
         <v>520</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F63" s="5"/>
-      <c r="G63" s="54" t="s">
+      <c r="F63" s="23">
+        <v>1011</v>
+      </c>
+      <c r="G63" s="36" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="64" ht="14.25" customHeight="1" spans="1:7">
-      <c r="A64" t="s">
+      <c r="A64" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B64" s="5">
+      <c r="B64" s="50">
         <v>5</v>
       </c>
-      <c r="C64" s="5">
+      <c r="C64" s="50">
         <v>35</v>
       </c>
-      <c r="D64" s="53">
-        <f>B64*C64</f>
+      <c r="D64" s="49">
+        <f t="shared" si="1"/>
         <v>175</v>
       </c>
       <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
-      <c r="G64" s="55"/>
+      <c r="F64" s="23"/>
+      <c r="G64" s="53"/>
     </row>
     <row r="65" ht="14.25" customHeight="1" spans="1:7">
-      <c r="A65" t="s">
+      <c r="A65" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="B65" s="5">
+      <c r="B65" s="50">
         <v>15</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C65" s="50">
         <v>15</v>
       </c>
-      <c r="D65" s="53">
-        <f>B65*C65</f>
+      <c r="D65" s="49">
+        <f t="shared" si="1"/>
         <v>225</v>
       </c>
       <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="55"/>
+      <c r="F65" s="23"/>
+      <c r="G65" s="53"/>
     </row>
     <row r="66" ht="14.25" customHeight="1" spans="1:7">
-      <c r="A66" s="6" t="s">
+      <c r="A66" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B66" s="5">
-        <v>1</v>
-      </c>
-      <c r="C66" s="5">
+      <c r="B66" s="50">
+        <v>1</v>
+      </c>
+      <c r="C66" s="50">
         <v>58</v>
       </c>
-      <c r="D66" s="53">
-        <f>B66*C66</f>
+      <c r="D66" s="49">
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="56"/>
+      <c r="F66" s="23"/>
+      <c r="G66" s="54"/>
     </row>
     <row r="67" ht="14.25" customHeight="1" spans="1:7">
       <c r="A67" t="s">
@@ -2951,15 +2960,15 @@
       <c r="C67" s="5">
         <v>813</v>
       </c>
-      <c r="D67" s="53">
-        <f>B67*C67</f>
+      <c r="D67" s="55">
+        <f t="shared" si="1"/>
         <v>813</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F67" s="5"/>
-      <c r="G67" s="57" t="s">
+      <c r="G67" s="36" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2973,13 +2982,13 @@
       <c r="C68" s="5">
         <v>58</v>
       </c>
-      <c r="D68" s="53">
-        <f>B68*C68</f>
+      <c r="D68" s="55">
+        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
-      <c r="G68" s="36"/>
+      <c r="G68" s="54"/>
     </row>
     <row r="69" ht="14.25" customHeight="1"/>
     <row r="70" ht="14.25" customHeight="1"/>
@@ -3926,7 +3935,7 @@
     <row r="1011" ht="14.25" customHeight="1"/>
     <row r="1012" ht="14.25" customHeight="1"/>
   </sheetData>
-  <mergeCells count="53">
+  <mergeCells count="52">
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="E5:E10"/>
     <mergeCell ref="E11:E12"/>
@@ -3979,7 +3988,6 @@
     <mergeCell ref="G33:G35"/>
     <mergeCell ref="G36:G37"/>
     <mergeCell ref="G52:G53"/>
-    <mergeCell ref="G67:G68"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup paperSize="1" orientation="landscape"/>
@@ -3990,10 +3998,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8421052631579" defaultRowHeight="14.4" outlineLevelCol="4"/>
@@ -4034,7 +4042,7 @@
         <v>109</v>
       </c>
       <c r="D3" s="4">
-        <f>PRODUCT(B3:C3)</f>
+        <f t="shared" ref="D3:D8" si="0">PRODUCT(B3:C3)</f>
         <v>327</v>
       </c>
     </row>
@@ -4049,7 +4057,7 @@
         <v>85</v>
       </c>
       <c r="D4" s="4">
-        <f>PRODUCT(B4:C4)</f>
+        <f t="shared" si="0"/>
         <v>85</v>
       </c>
     </row>
@@ -4064,7 +4072,7 @@
         <v>520</v>
       </c>
       <c r="D5" s="4">
-        <f>PRODUCT(B5:C5)</f>
+        <f t="shared" si="0"/>
         <v>520</v>
       </c>
       <c r="E5" s="8" t="s">
@@ -4082,7 +4090,7 @@
         <v>35</v>
       </c>
       <c r="D6" s="4">
-        <f>PRODUCT(B6:C6)</f>
+        <f t="shared" si="0"/>
         <v>175</v>
       </c>
     </row>
@@ -4097,7 +4105,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="4">
-        <f>PRODUCT(B7:C7)</f>
+        <f t="shared" si="0"/>
         <v>225</v>
       </c>
     </row>
@@ -4112,7 +4120,7 @@
         <v>95</v>
       </c>
       <c r="D8" s="4">
-        <f>PRODUCT(B8:C8)</f>
+        <f t="shared" si="0"/>
         <v>95</v>
       </c>
     </row>
@@ -4226,7 +4234,7 @@
         <v>295</v>
       </c>
       <c r="D18" s="5">
-        <f t="shared" ref="D18:D54" si="0">C18*B18</f>
+        <f t="shared" ref="D18:D29" si="1">C18*B18</f>
         <v>295</v>
       </c>
     </row>
@@ -4241,7 +4249,7 @@
         <v>329</v>
       </c>
       <c r="D19" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>329</v>
       </c>
     </row>
@@ -4256,7 +4264,7 @@
         <v>195</v>
       </c>
       <c r="D20" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>195</v>
       </c>
     </row>
@@ -4271,7 +4279,7 @@
         <v>195</v>
       </c>
       <c r="D21" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>195</v>
       </c>
     </row>
@@ -4286,7 +4294,7 @@
         <v>294</v>
       </c>
       <c r="D22" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>294</v>
       </c>
     </row>
@@ -4301,7 +4309,7 @@
         <v>345</v>
       </c>
       <c r="D23" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>345</v>
       </c>
     </row>
@@ -4316,7 +4324,7 @@
         <v>494</v>
       </c>
       <c r="D24" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>494</v>
       </c>
     </row>
@@ -4331,7 +4339,7 @@
         <v>395</v>
       </c>
       <c r="D25" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>395</v>
       </c>
     </row>
@@ -4346,7 +4354,7 @@
         <v>180</v>
       </c>
       <c r="D26" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>180</v>
       </c>
     </row>
@@ -4361,7 +4369,7 @@
         <v>255</v>
       </c>
       <c r="D27" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>255</v>
       </c>
     </row>
@@ -4376,161 +4384,161 @@
         <v>375</v>
       </c>
       <c r="D28" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>375</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" t="s">
+      <c r="A29" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="5">
+        <v>1</v>
+      </c>
+      <c r="C29" s="5">
+        <v>58</v>
+      </c>
+      <c r="D29" s="5">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="5">
-        <v>1</v>
-      </c>
-      <c r="C29" s="5">
+      <c r="B30" s="5">
+        <v>1</v>
+      </c>
+      <c r="C30" s="5">
         <v>254</v>
       </c>
-      <c r="D29" s="5">
-        <f t="shared" si="0"/>
+      <c r="D30" s="5">
+        <f t="shared" ref="D30:D59" si="2">C30*B30</f>
         <v>254</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="7" t="s">
+    <row r="31" spans="1:4">
+      <c r="A31" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="B30" s="5">
-        <v>1</v>
-      </c>
-      <c r="C30" s="5">
+      <c r="B31" s="5">
+        <v>1</v>
+      </c>
+      <c r="C31" s="5">
         <v>195</v>
       </c>
-      <c r="D30" s="5">
-        <f t="shared" si="0"/>
+      <c r="D31" s="5">
+        <f t="shared" si="2"/>
         <v>195</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>71</v>
-      </c>
-      <c r="B31" s="5">
-        <v>1</v>
-      </c>
-      <c r="C31" s="5">
-        <v>395</v>
-      </c>
-      <c r="D31" s="5">
-        <f t="shared" si="0"/>
-        <v>395</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B32" s="5">
         <v>1</v>
       </c>
       <c r="C32" s="5">
-        <v>275</v>
+        <v>395</v>
       </c>
       <c r="D32" s="5">
-        <f t="shared" si="0"/>
-        <v>275</v>
+        <f t="shared" si="2"/>
+        <v>395</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B33" s="5">
         <v>1</v>
       </c>
       <c r="C33" s="5">
-        <v>215</v>
+        <v>275</v>
       </c>
       <c r="D33" s="5">
-        <f t="shared" si="0"/>
-        <v>215</v>
+        <f t="shared" si="2"/>
+        <v>275</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34" s="5">
         <v>1</v>
       </c>
       <c r="C34" s="5">
-        <v>285</v>
+        <v>215</v>
       </c>
       <c r="D34" s="5">
-        <f t="shared" si="0"/>
-        <v>285</v>
+        <f t="shared" si="2"/>
+        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35" s="5">
         <v>1</v>
       </c>
       <c r="C35" s="5">
-        <v>245</v>
+        <v>285</v>
       </c>
       <c r="D35" s="5">
-        <f t="shared" si="0"/>
-        <v>245</v>
+        <f t="shared" si="2"/>
+        <v>285</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B36" s="5">
         <v>1</v>
       </c>
       <c r="C36" s="5">
-        <v>308</v>
+        <v>245</v>
       </c>
       <c r="D36" s="5">
-        <f t="shared" si="0"/>
-        <v>308</v>
+        <f t="shared" si="2"/>
+        <v>245</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="5">
+        <v>1</v>
+      </c>
+      <c r="C37" s="5">
+        <v>308</v>
+      </c>
+      <c r="D37" s="5">
+        <f t="shared" si="2"/>
+        <v>308</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
         <v>77</v>
       </c>
-      <c r="B37" s="5">
-        <v>1</v>
-      </c>
-      <c r="C37" s="5">
+      <c r="B38" s="5">
+        <v>1</v>
+      </c>
+      <c r="C38" s="5">
         <v>315</v>
       </c>
-      <c r="D37" s="5">
-        <f t="shared" si="0"/>
+      <c r="D38" s="5">
+        <f t="shared" si="2"/>
         <v>315</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38" s="5">
-        <v>1</v>
-      </c>
-      <c r="C38" s="5">
-        <v>95</v>
-      </c>
-      <c r="D38" s="5">
-        <f t="shared" si="0"/>
-        <v>95</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -4538,223 +4546,221 @@
         <v>1</v>
       </c>
       <c r="C39" s="5">
-        <v>203</v>
+        <v>339</v>
       </c>
       <c r="D39" s="5">
-        <f t="shared" si="0"/>
-        <v>203</v>
-      </c>
-      <c r="E39" s="12"/>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" t="s">
-        <v>79</v>
+        <f t="shared" si="2"/>
+        <v>339</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="B40" s="5">
         <v>1</v>
       </c>
       <c r="C40" s="5">
-        <v>255</v>
+        <v>58</v>
       </c>
       <c r="D40" s="5">
-        <f t="shared" si="0"/>
-        <v>255</v>
-      </c>
-      <c r="E40" s="12"/>
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B41" s="5">
         <v>1</v>
       </c>
       <c r="C41" s="5">
-        <v>359</v>
+        <v>203</v>
       </c>
       <c r="D41" s="5">
-        <f t="shared" si="0"/>
-        <v>359</v>
+        <f t="shared" si="2"/>
+        <v>203</v>
       </c>
       <c r="E41" s="12"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B42" s="5">
         <v>1</v>
       </c>
       <c r="C42" s="5">
-        <v>219</v>
+        <v>255</v>
       </c>
       <c r="D42" s="5">
-        <f t="shared" si="0"/>
-        <v>219</v>
+        <f t="shared" si="2"/>
+        <v>255</v>
       </c>
       <c r="E42" s="12"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B43" s="5">
         <v>1</v>
       </c>
       <c r="C43" s="5">
-        <v>247</v>
+        <v>359</v>
       </c>
       <c r="D43" s="5">
-        <f t="shared" si="0"/>
-        <v>247</v>
+        <f t="shared" si="2"/>
+        <v>359</v>
       </c>
       <c r="E43" s="12"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B44" s="5">
         <v>1</v>
       </c>
       <c r="C44" s="5">
-        <v>280</v>
+        <v>219</v>
       </c>
       <c r="D44" s="5">
-        <f t="shared" si="0"/>
-        <v>280</v>
+        <f t="shared" si="2"/>
+        <v>219</v>
       </c>
       <c r="E44" s="12"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B45" s="5">
         <v>1</v>
       </c>
       <c r="C45" s="5">
-        <v>194</v>
+        <v>247</v>
       </c>
       <c r="D45" s="5">
-        <f t="shared" si="0"/>
-        <v>194</v>
+        <f t="shared" si="2"/>
+        <v>247</v>
       </c>
       <c r="E45" s="12"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B46" s="5">
         <v>1</v>
       </c>
       <c r="C46" s="5">
-        <v>384</v>
+        <v>280</v>
       </c>
       <c r="D46" s="5">
-        <f t="shared" si="0"/>
-        <v>384</v>
+        <f t="shared" si="2"/>
+        <v>280</v>
       </c>
       <c r="E46" s="12"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B47" s="5">
         <v>1</v>
       </c>
       <c r="C47" s="5">
-        <v>233</v>
+        <v>194</v>
       </c>
       <c r="D47" s="5">
-        <f t="shared" si="0"/>
-        <v>233</v>
+        <f t="shared" si="2"/>
+        <v>194</v>
       </c>
       <c r="E47" s="12"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B48" s="5">
         <v>1</v>
       </c>
       <c r="C48" s="5">
-        <v>233</v>
+        <v>384</v>
       </c>
       <c r="D48" s="5">
-        <f t="shared" si="0"/>
-        <v>233</v>
+        <f t="shared" si="2"/>
+        <v>384</v>
       </c>
       <c r="E48" s="12"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B49" s="5">
         <v>1</v>
       </c>
       <c r="C49" s="5">
-        <v>181</v>
+        <v>233</v>
       </c>
       <c r="D49" s="5">
-        <f t="shared" si="0"/>
-        <v>181</v>
+        <f t="shared" si="2"/>
+        <v>233</v>
       </c>
       <c r="E49" s="12"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="5">
+        <v>1</v>
+      </c>
+      <c r="C50" s="5">
+        <v>233</v>
+      </c>
+      <c r="D50" s="5">
+        <f t="shared" si="2"/>
+        <v>233</v>
+      </c>
+      <c r="E50" s="12"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
         <v>89</v>
       </c>
-      <c r="B50" s="5">
-        <v>1</v>
-      </c>
-      <c r="C50" s="5">
+      <c r="B51" s="5">
+        <v>1</v>
+      </c>
+      <c r="C51" s="5">
+        <v>181</v>
+      </c>
+      <c r="D51" s="5">
+        <f t="shared" si="2"/>
+        <v>181</v>
+      </c>
+      <c r="E51" s="12"/>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>90</v>
+      </c>
+      <c r="B52" s="5">
+        <v>1</v>
+      </c>
+      <c r="C52" s="5">
         <v>212</v>
       </c>
-      <c r="D50" s="5">
-        <f t="shared" si="0"/>
+      <c r="D52" s="5">
+        <f t="shared" si="2"/>
         <v>212</v>
       </c>
-      <c r="E50" s="12"/>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B51" s="5">
-        <v>1</v>
-      </c>
-      <c r="C51" s="5">
-        <v>268</v>
-      </c>
-      <c r="D51" s="5">
-        <f t="shared" si="0"/>
-        <v>268</v>
-      </c>
-      <c r="E51" s="12"/>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B52" s="5">
-        <v>1</v>
-      </c>
-      <c r="C52" s="5">
-        <v>195</v>
-      </c>
-      <c r="D52" s="5">
-        <f t="shared" si="0"/>
-        <v>195</v>
-      </c>
-      <c r="E52" s="13"/>
-    </row>
-    <row r="53" ht="15.6" spans="1:5">
+      <c r="E52" s="12"/>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" s="7" t="s">
         <v>91</v>
       </c>
@@ -4762,47 +4768,127 @@
         <v>1</v>
       </c>
       <c r="C53" s="5">
+        <v>203</v>
+      </c>
+      <c r="D53" s="5">
+        <f t="shared" si="2"/>
+        <v>203</v>
+      </c>
+      <c r="E53" s="12"/>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B54" s="5">
+        <v>1</v>
+      </c>
+      <c r="C54" s="5">
+        <v>248</v>
+      </c>
+      <c r="D54" s="5">
+        <f t="shared" si="2"/>
+        <v>248</v>
+      </c>
+      <c r="E54" s="12"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55" s="5">
+        <v>1</v>
+      </c>
+      <c r="C55" s="5">
+        <v>198</v>
+      </c>
+      <c r="D55" s="5">
+        <f t="shared" si="2"/>
+        <v>198</v>
+      </c>
+      <c r="E55" s="12"/>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B56" s="5">
+        <v>1</v>
+      </c>
+      <c r="C56" s="5">
+        <v>209</v>
+      </c>
+      <c r="D56" s="5">
+        <f t="shared" si="2"/>
+        <v>209</v>
+      </c>
+      <c r="E56" s="12"/>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" s="5">
+        <v>1</v>
+      </c>
+      <c r="C57" s="5">
+        <v>195</v>
+      </c>
+      <c r="D57" s="5">
+        <f t="shared" si="2"/>
+        <v>195</v>
+      </c>
+      <c r="E57" s="13"/>
+    </row>
+    <row r="58" ht="15.6" spans="1:5">
+      <c r="A58" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58" s="5">
+        <v>1</v>
+      </c>
+      <c r="C58" s="5">
         <v>319</v>
       </c>
-      <c r="D53" s="5">
-        <f t="shared" si="0"/>
+      <c r="D58" s="5">
+        <f t="shared" si="2"/>
         <v>319</v>
       </c>
-      <c r="E53" s="14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="6" t="s">
+      <c r="E58" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B54" s="5">
-        <v>1</v>
-      </c>
-      <c r="C54" s="5">
+      <c r="B59" s="5">
+        <v>1</v>
+      </c>
+      <c r="C59" s="5">
         <v>85</v>
       </c>
-      <c r="D54" s="5">
-        <f t="shared" si="0"/>
+      <c r="D59" s="5">
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="3:4">
-      <c r="C55" s="9" t="s">
+    <row r="60" spans="3:4">
+      <c r="C60" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D55" s="11">
-        <f>SUM(D18:D54)</f>
-        <v>9801</v>
-      </c>
-    </row>
-    <row r="56" spans="3:4">
-      <c r="C56" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D56" s="16">
-        <f>D55+D16+D9</f>
-        <v>13928</v>
+      <c r="D60" s="11">
+        <f>SUM(D18:D59)</f>
+        <v>10751</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4">
+      <c r="C61" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D61" s="16">
+        <f>D60+D16+D9</f>
+        <v>14878</v>
       </c>
     </row>
   </sheetData>
@@ -4828,178 +4914,178 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" t="s">
         <v>101</v>
-      </c>
-      <c r="B6" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B16" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B18" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B20" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B22" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
U: IC, PR, Supp
Changed prospect new scents; Updated order status; updated supply logs
</commit_message>
<xml_diff>
--- a/Supplies.xlsx
+++ b/Supplies.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8952" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="8952"/>
   </bookViews>
   <sheets>
     <sheet name="Capital Estimate (Inspired)" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="131">
   <si>
     <t>Quantity</t>
   </si>
@@ -172,7 +172,10 @@
     <t>125mL FO - Parfum Aromatics Co.</t>
   </si>
   <si>
-    <t>Dear Polly</t>
+    <t>Dear Polly, Lys Mediterranee</t>
+  </si>
+  <si>
+    <t>Gaiac 10, Vetyver, Eternity Now</t>
   </si>
   <si>
     <t>Qty</t>
@@ -1316,23 +1319,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1817,8 +1820,8 @@
   <sheetPr/>
   <dimension ref="A1:G1012"/>
   <sheetViews>
-    <sheetView zoomScale="82" zoomScaleNormal="82" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63:F66"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63:E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4298245614035" defaultRowHeight="15" customHeight="1" outlineLevelCol="6"/>
@@ -2761,43 +2764,43 @@
     </row>
     <row r="56" ht="14.25" customHeight="1"/>
     <row r="57" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A57" s="50" t="s">
+      <c r="A57" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B57" s="51">
+      <c r="B57" s="9">
         <v>50</v>
       </c>
-      <c r="C57" s="51">
+      <c r="C57" s="9">
         <v>20</v>
       </c>
-      <c r="D57" s="50">
-        <f t="shared" ref="D57:D68" si="1">B57*C57</f>
+      <c r="D57" s="22">
+        <f t="shared" ref="D57:D70" si="1">B57*C57</f>
         <v>1000</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F57" s="52">
+      <c r="F57" s="50">
         <f>996+105+22</f>
         <v>1123</v>
       </c>
     </row>
     <row r="58" ht="14.25" customHeight="1" spans="1:6">
-      <c r="A58" s="53" t="s">
+      <c r="A58" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B58" s="51">
-        <v>1</v>
-      </c>
-      <c r="C58" s="51">
+      <c r="B58" s="9">
+        <v>1</v>
+      </c>
+      <c r="C58" s="9">
         <v>105</v>
       </c>
-      <c r="D58" s="50">
+      <c r="D58" s="22">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
       <c r="E58" s="5"/>
-      <c r="F58" s="52"/>
+      <c r="F58" s="50"/>
     </row>
     <row r="59" ht="14.25" customHeight="1" spans="1:6">
       <c r="A59" s="22" t="s">
@@ -2816,7 +2819,7 @@
       <c r="E59" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F59" s="52">
+      <c r="F59" s="50">
         <f>92+58+3</f>
         <v>153</v>
       </c>
@@ -2836,7 +2839,7 @@
         <v>58</v>
       </c>
       <c r="E60" s="5"/>
-      <c r="F60" s="52"/>
+      <c r="F60" s="50"/>
     </row>
     <row r="61" ht="14.25" customHeight="1" spans="1:6">
       <c r="A61" s="22" t="s">
@@ -2855,7 +2858,7 @@
       <c r="E61" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F61" s="52">
+      <c r="F61" s="50">
         <f>690+45+15</f>
         <v>750</v>
       </c>
@@ -2875,7 +2878,7 @@
         <v>125</v>
       </c>
       <c r="E62" s="5"/>
-      <c r="F62" s="52"/>
+      <c r="F62" s="50"/>
     </row>
     <row r="63" ht="14.25" customHeight="1" spans="1:7">
       <c r="A63" s="22" t="s">
@@ -2918,7 +2921,7 @@
       </c>
       <c r="E64" s="5"/>
       <c r="F64" s="26"/>
-      <c r="G64" s="54"/>
+      <c r="G64" s="51"/>
     </row>
     <row r="65" ht="14.25" customHeight="1" spans="1:7">
       <c r="A65" s="22" t="s">
@@ -2936,7 +2939,7 @@
       </c>
       <c r="E65" s="5"/>
       <c r="F65" s="26"/>
-      <c r="G65" s="54"/>
+      <c r="G65" s="51"/>
     </row>
     <row r="66" ht="14.25" customHeight="1" spans="1:7">
       <c r="A66" s="12" t="s">
@@ -2954,50 +2957,92 @@
       </c>
       <c r="E66" s="5"/>
       <c r="F66" s="26"/>
-      <c r="G66" s="55"/>
+      <c r="G66" s="52"/>
     </row>
     <row r="67" ht="14.25" customHeight="1" spans="1:7">
-      <c r="A67" t="s">
+      <c r="A67" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="B67" s="5">
-        <v>1</v>
-      </c>
-      <c r="C67" s="5">
-        <v>813</v>
-      </c>
-      <c r="D67" s="56">
+      <c r="B67" s="54">
+        <v>1</v>
+      </c>
+      <c r="C67" s="54">
+        <f>813+821</f>
+        <v>1634</v>
+      </c>
+      <c r="D67" s="53">
         <f t="shared" si="1"/>
-        <v>813</v>
+        <v>1634</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F67" s="5"/>
+      <c r="F67" s="26">
+        <f>1270+8+26</f>
+        <v>1304</v>
+      </c>
       <c r="G67" s="39" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1" spans="1:7">
-      <c r="A68" s="6" t="s">
+      <c r="A68" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="B68" s="5">
-        <v>1</v>
-      </c>
-      <c r="C68" s="5">
+      <c r="B68" s="54">
+        <v>1</v>
+      </c>
+      <c r="C68" s="54">
         <v>58</v>
       </c>
-      <c r="D68" s="56">
+      <c r="D68" s="53">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="55"/>
-    </row>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
+      <c r="F68" s="26"/>
+      <c r="G68" s="52"/>
+    </row>
+    <row r="69" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A69" t="s">
+        <v>23</v>
+      </c>
+      <c r="B69" s="5">
+        <v>1</v>
+      </c>
+      <c r="C69" s="5">
+        <f>650+520+520</f>
+        <v>1690</v>
+      </c>
+      <c r="D69" s="56">
+        <f t="shared" si="1"/>
+        <v>1690</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F69" s="5"/>
+      <c r="G69" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="70" ht="14.25" customHeight="1" spans="1:6">
+      <c r="A70" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B70" s="5">
+        <v>1</v>
+      </c>
+      <c r="C70" s="5">
+        <v>58</v>
+      </c>
+      <c r="D70" s="56">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+    </row>
     <row r="71" ht="14.25" customHeight="1"/>
     <row r="72" ht="14.25" customHeight="1"/>
     <row r="73" ht="14.25" customHeight="1"/>
@@ -3941,7 +3986,7 @@
     <row r="1011" ht="14.25" customHeight="1"/>
     <row r="1012" ht="14.25" customHeight="1"/>
   </sheetData>
-  <mergeCells count="52">
+  <mergeCells count="54">
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="E5:E10"/>
     <mergeCell ref="E11:E12"/>
@@ -3966,6 +4011,7 @@
     <mergeCell ref="E61:E62"/>
     <mergeCell ref="E63:E66"/>
     <mergeCell ref="E67:E68"/>
+    <mergeCell ref="E69:E70"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="F5:F10"/>
     <mergeCell ref="F11:F12"/>
@@ -3990,6 +4036,7 @@
     <mergeCell ref="F61:F62"/>
     <mergeCell ref="F63:F66"/>
     <mergeCell ref="F67:F68"/>
+    <mergeCell ref="F69:F70"/>
     <mergeCell ref="G26:G27"/>
     <mergeCell ref="G33:G35"/>
     <mergeCell ref="G36:G37"/>
@@ -4006,7 +4053,7 @@
   <sheetPr/>
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
@@ -4021,7 +4068,7 @@
   <sheetData>
     <row r="1" spans="2:5">
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -4041,7 +4088,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B3" s="4">
         <v>3</v>
@@ -4094,7 +4141,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B6" s="8">
         <v>5</v>
@@ -4110,7 +4157,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B7" s="8">
         <v>15</v>
@@ -4143,7 +4190,7 @@
     <row r="9" spans="2:5">
       <c r="B9" s="4"/>
       <c r="C9" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D9" s="14">
         <f>SUM(D3:D8)</f>
@@ -4165,7 +4212,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B12" s="5">
         <v>3</v>
@@ -4179,7 +4226,7 @@
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -4200,7 +4247,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B14" s="5">
         <v>1</v>
@@ -4216,7 +4263,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B15" s="5">
         <v>30</v>
@@ -4233,7 +4280,7 @@
     <row r="16" spans="1:5">
       <c r="A16" s="1"/>
       <c r="C16" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D16" s="16">
         <f>SUM(D12:D15)</f>
@@ -4243,12 +4290,12 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B18" s="5">
         <v>1</v>
@@ -4257,14 +4304,14 @@
         <v>295</v>
       </c>
       <c r="D18" s="5">
-        <f t="shared" ref="D18:D29" si="1">C18*B18</f>
+        <f t="shared" ref="D18:D40" si="1">C18*B18</f>
         <v>295</v>
       </c>
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B19" s="5">
         <v>1</v>
@@ -4280,7 +4327,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B20" s="5">
         <v>1</v>
@@ -4296,7 +4343,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B21" s="5">
         <v>1</v>
@@ -4312,7 +4359,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B22" s="5">
         <v>1</v>
@@ -4328,7 +4375,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B23" s="5">
         <v>1</v>
@@ -4344,7 +4391,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B24" s="5">
         <v>1</v>
@@ -4360,7 +4407,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B25" s="5">
         <v>1</v>
@@ -4376,7 +4423,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B26" s="5">
         <v>1</v>
@@ -4392,7 +4439,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B27" s="5">
         <v>1</v>
@@ -4408,7 +4455,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B28" s="5">
         <v>1</v>
@@ -4440,7 +4487,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B30" s="5">
         <v>1</v>
@@ -4449,14 +4496,14 @@
         <v>254</v>
       </c>
       <c r="D30" s="5">
-        <f>C30*B30</f>
+        <f t="shared" si="1"/>
         <v>254</v>
       </c>
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B31" s="5">
         <v>1</v>
@@ -4465,14 +4512,14 @@
         <v>195</v>
       </c>
       <c r="D31" s="5">
-        <f>C31*B31</f>
+        <f t="shared" si="1"/>
         <v>195</v>
       </c>
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B32" s="5">
         <v>1</v>
@@ -4481,14 +4528,14 @@
         <v>395</v>
       </c>
       <c r="D32" s="5">
-        <f>C32*B32</f>
+        <f t="shared" si="1"/>
         <v>395</v>
       </c>
       <c r="E32" s="5"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B33" s="5">
         <v>1</v>
@@ -4497,14 +4544,14 @@
         <v>275</v>
       </c>
       <c r="D33" s="5">
-        <f>C33*B33</f>
+        <f t="shared" si="1"/>
         <v>275</v>
       </c>
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B34" s="5">
         <v>1</v>
@@ -4513,14 +4560,14 @@
         <v>215</v>
       </c>
       <c r="D34" s="5">
-        <f>C34*B34</f>
+        <f t="shared" si="1"/>
         <v>215</v>
       </c>
       <c r="E34" s="5"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B35" s="5">
         <v>1</v>
@@ -4529,14 +4576,14 @@
         <v>285</v>
       </c>
       <c r="D35" s="5">
-        <f>C35*B35</f>
+        <f t="shared" si="1"/>
         <v>285</v>
       </c>
       <c r="E35" s="5"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B36" s="5">
         <v>1</v>
@@ -4545,14 +4592,14 @@
         <v>245</v>
       </c>
       <c r="D36" s="5">
-        <f>C36*B36</f>
+        <f t="shared" si="1"/>
         <v>245</v>
       </c>
       <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B37" s="5">
         <v>1</v>
@@ -4561,14 +4608,14 @@
         <v>308</v>
       </c>
       <c r="D37" s="5">
-        <f>C37*B37</f>
+        <f t="shared" si="1"/>
         <v>308</v>
       </c>
       <c r="E37" s="5"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B38" s="5">
         <v>1</v>
@@ -4577,14 +4624,14 @@
         <v>315</v>
       </c>
       <c r="D38" s="5">
-        <f>C38*B38</f>
+        <f t="shared" si="1"/>
         <v>315</v>
       </c>
       <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B39" s="5">
         <v>1</v>
@@ -4593,14 +4640,14 @@
         <v>339</v>
       </c>
       <c r="D39" s="5">
-        <f>C39*B39</f>
+        <f t="shared" si="1"/>
         <v>339</v>
       </c>
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B40" s="5">
         <v>1</v>
@@ -4609,7 +4656,7 @@
         <v>299</v>
       </c>
       <c r="D40" s="5">
-        <f>C40*B40</f>
+        <f t="shared" si="1"/>
         <v>299</v>
       </c>
       <c r="E40" s="5"/>
@@ -4632,7 +4679,7 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B42" s="5">
         <v>1</v>
@@ -4649,7 +4696,7 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B43" s="5">
         <v>1</v>
@@ -4666,7 +4713,7 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B44" s="5">
         <v>1</v>
@@ -4683,7 +4730,7 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B45" s="5">
         <v>1</v>
@@ -4700,7 +4747,7 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B46" s="5">
         <v>1</v>
@@ -4717,7 +4764,7 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B47" s="5">
         <v>1</v>
@@ -4734,7 +4781,7 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B48" s="5">
         <v>1</v>
@@ -4751,7 +4798,7 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B49" s="5">
         <v>1</v>
@@ -4768,7 +4815,7 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B50" s="5">
         <v>1</v>
@@ -4785,7 +4832,7 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B51" s="5">
         <v>1</v>
@@ -4802,7 +4849,7 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B52" s="5">
         <v>1</v>
@@ -4819,7 +4866,7 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B53" s="5">
         <v>1</v>
@@ -4836,7 +4883,7 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="15" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B54" s="5">
         <v>1</v>
@@ -4853,7 +4900,7 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="15" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B55" s="5">
         <v>1</v>
@@ -4870,7 +4917,7 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B56" s="5">
         <v>1</v>
@@ -4887,7 +4934,7 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="15" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B57" s="5">
         <v>1</v>
@@ -4921,7 +4968,7 @@
     </row>
     <row r="59" ht="15.6" spans="1:6">
       <c r="A59" s="15" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B59" s="5">
         <v>1</v>
@@ -4935,7 +4982,7 @@
       </c>
       <c r="E59" s="5"/>
       <c r="F59" s="19" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -4956,7 +5003,7 @@
     </row>
     <row r="61" spans="3:5">
       <c r="C61" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D61" s="16">
         <f>SUM(D18:D60)</f>
@@ -4966,7 +5013,7 @@
     </row>
     <row r="62" spans="3:5">
       <c r="C62" s="20" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D62" s="21">
         <f>D61+D16+D9</f>
@@ -5000,178 +5047,178 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
         <v>103</v>
-      </c>
-      <c r="B3" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B11" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B13" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B17" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B18" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" t="s">
         <v>123</v>
-      </c>
-      <c r="B19" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B20" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B21" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B22" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>